<commit_message>
Adding support for user creation and for setting the rest of the user fields
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Team-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75C3FC44-A5BE-4B53-85FF-01AAA14873A0}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DDC0857-7854-4A25-A873-B73F8DDC2184}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -31,23 +31,74 @@
     <t>Users will be found by Username. Leave a field empty to ignore it.</t>
   </si>
   <si>
-    <t>This field is not incremental, the value will be fully replaces. To clear this field, send NONE</t>
-  </si>
-  <si>
-    <t>This field is not incremental, the value will be fully replaces.</t>
-  </si>
-  <si>
     <t>Teams Managed (not incremental)</t>
   </si>
   <si>
     <t>Roles (not incremental)</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>API Service Account</t>
+  </si>
+  <si>
+    <t>Set to true if creating a new user to set it as an API service account (this field is ignored for existing users)</t>
+  </si>
+  <si>
+    <t>This field is not incremental, the value will be fully replaced. To clear this field, send NONE</t>
+  </si>
+  <si>
+    <t>Empty values will be ignored. To clear this field, send NONE</t>
+  </si>
+  <si>
+    <t>Login Enabled</t>
+  </si>
+  <si>
+    <t>Custom 1</t>
+  </si>
+  <si>
+    <t>Custom 2</t>
+  </si>
+  <si>
+    <t>Custom 3</t>
+  </si>
+  <si>
+    <t>Custom 4</t>
+  </si>
+  <si>
+    <t>Custom 5</t>
+  </si>
+  <si>
+    <t>This field will be set to 'success' if the import is successful, otherwise, it will contain an error message</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Restrict Login Ips</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +126,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,11 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,71 +479,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A3:D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
-    <col min="17" max="24" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="40" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.7109375" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="59.85546875" customWidth="1"/>
+    <col min="6" max="15" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="42" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="C8" s="3"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="Q8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improving field descriptions on Excel and adding TODOs for unsupported account types
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Team-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DDC0857-7854-4A25-A873-B73F8DDC2184}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF6BCD0B-F6F9-4CC6-AC98-F25C0B6030F1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Set to true if creating a new user to set it as an API service account (this field is ignored for existing users)</t>
   </si>
   <si>
-    <t>This field is not incremental, the value will be fully replaced. To clear this field, send NONE</t>
-  </si>
-  <si>
     <t>Empty values will be ignored. To clear this field, send NONE</t>
   </si>
   <si>
@@ -82,16 +79,28 @@
     <t>Status</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Restrict Login Ips</t>
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>First Name*</t>
+  </si>
+  <si>
+    <t>Last Name*</t>
+  </si>
+  <si>
+    <t>Empty values will be ignored. For new users, this is mandatory</t>
+  </si>
+  <si>
+    <t>This field is not incremental, the value will be fully replaced. This field is mandatory - setting this to NONE will throw an error</t>
+  </si>
+  <si>
+    <t>This is combined with the Teams field and is not incremental, the value will be fully replaced. To clear this field, send NONE.</t>
+  </si>
+  <si>
+    <t>This is combined with the Teams Managed field and is not incremental, the value will be fully replaced. To clear this field, send NONE.</t>
   </si>
 </sst>
 </file>
@@ -481,7 +490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -490,7 +501,9 @@
     <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="59.85546875" customWidth="1"/>
     <col min="6" max="15" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="135.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="111.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="80.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="90.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="42" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -501,58 +514,58 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -560,16 +573,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -581,25 +594,25 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>1</v>
@@ -611,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding support for API accounts and initializing API credentials
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Team-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF6BCD0B-F6F9-4CC6-AC98-F25C0B6030F1}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CADF3288-ED30-4CD3-B3CA-54F4EA630D9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -101,13 +101,19 @@
   </si>
   <si>
     <t>This is combined with the Teams Managed field and is not incremental, the value will be fully replaced. To clear this field, send NONE.</t>
+  </si>
+  <si>
+    <t>API ID</t>
+  </si>
+  <si>
+    <t>API Secret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +149,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,17 +175,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +526,7 @@
     <col min="27" max="42" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -568,7 +585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -626,18 +643,27 @@
       <c r="S2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>

</xml_diff>